<commit_message>
All iterations for session 4 assignment
</commit_message>
<xml_diff>
--- a/Session-4/ExperinmentLog.xlsx
+++ b/Session-4/ExperinmentLog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t xml:space="preserve">Model No and version</t>
   </si>
@@ -72,10 +72,157 @@
   </si>
   <si>
     <t xml:space="preserve">Similar case of over fitting with lower no of params
-Epoch 1/20
-60000/60000 [==============================] - 11s 189us/step - loss: 0.1848 - acc: 0.9447 - val_loss: 0.0637 - val_acc: 0.9805
-Epoch 20/20
-60000/60000 [==============================] - 11s 181us/step - loss: 0.0065 - acc: 0.9979 - val_loss: 0.0572 - val_acc: 0.9895</t>
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_3rdDNN-v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Batch Normalization for Assignment4-2ndDNN-v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increased total Params; Lower over fitting though still visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_3rdDNN-v1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding Batch normalization in version 1 model for all layers
+Changing layer for lower total param
+Adding drop out twice of 0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Params under 15K; Over fitting significantly lower with dropout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_3rdDNN-v2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">For Version 2 of model of 3</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> DNN: Adding Batch normalization to call cnn layers
+Changing layer for lower total param
+Adding drop out twice of 0.2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Params under 15K; Over fitting significantly lower, still visible though
+Validation acc significantly increased; loss reduction also better</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_3rdDNN-v3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slight over fitting, overall perfomance seems better</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_4thDNN-v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch size 64
+  Epoch 30
+  Learning rate schedule with starting lr .001 and scheduler defined as example from session material
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training for model improved significantly; low  overfitting; further improvisation on LR  and increased epoch can help get suitable accuracy
+Val acc: 9883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_4thDNN-v1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch 128
+Epochh 50
+LR .005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val acc above .9909; Moderate over fitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_4thDNN-v1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LR .01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val acc above .9904; Moderate over fitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_4thDNN-v2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val acc above .9924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_4thDNN-v2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch size 128
+  Epoch 50
+  Learning rate schedule with starting lr .01 and scheduler defined as example from session material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val acc above .9919; overall training faster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LR .008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val acc: .9905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_4thDNN-v3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch size 128
+  Epoch 50
+  Learning rate schedule with starting lr .008 and scheduler defined as example from session material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val acc above .9925; Moderate over fitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4_4thDNN-v3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base LR .01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val acc above .9918; Moderate over fitting; not much change from previous model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment4-4thDNN-v3.4-SGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With sgd optimizer and base LR of .1 and LR scheduler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val acc above .9913; low/no over fitting</t>
   </si>
 </sst>
 </file>
@@ -85,7 +232,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -109,6 +256,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -163,13 +317,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -257,40 +415,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="bottomLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="46.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="67.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="46.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="67.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="3" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AMJ1" s="0"/>
@@ -308,10 +466,10 @@
       <c r="D2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -328,10 +486,10 @@
       <c r="D3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -348,14 +506,14 @@
       <c r="D4" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -368,19 +526,271 @@
       <c r="D5" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>15180</v>
+      </c>
       <c r="C6" s="1" t="n">
         <v>32</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>14823</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>14384</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="47" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>14536</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>14823</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>14823</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>14823</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>14384</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>14384</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>14384</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>14536</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>14536</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>14536</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>